<commit_message>
cambios del convenio, css de multinacional y reparar error del name de cotizacion
</commit_message>
<xml_diff>
--- a/convenios/caracas.xlsx
+++ b/convenios/caracas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16560" tabRatio="500" firstSheet="6" activeTab="8"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16560" tabRatio="500" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_tipo_carro" sheetId="6" state="hidden" r:id="rId1"/>
@@ -15,11 +15,11 @@
     <sheet name="tbl_plan_detalle" sheetId="16" state="hidden" r:id="rId6"/>
     <sheet name="tbl_tasa_casco" sheetId="8" r:id="rId7"/>
     <sheet name="tbl_clasificacion" sheetId="9" r:id="rId8"/>
-    <sheet name="tbl_suma_asegurada" sheetId="19" r:id="rId9"/>
+    <sheet name="tbl_clasificacion_ma" sheetId="19" r:id="rId9"/>
     <sheet name="tbl_re_tipo_cob_as" sheetId="4" r:id="rId10"/>
     <sheet name="tbl_grua" sheetId="18" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1137,13 +1137,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="9"/>
-  </sheetPr>
   <dimension ref="A3:J93"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -3501,13 +3498,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="9"/>
-  </sheetPr>
   <dimension ref="A3:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -5046,13 +5040,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="9"/>
-  </sheetPr>
   <dimension ref="B3:G194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -8190,13 +8181,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="9"/>
-  </sheetPr>
   <dimension ref="B3:F385"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -10910,13 +10898,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="9"/>
-  </sheetPr>
   <dimension ref="B3:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -10953,10 +10938,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="8">
-        <v>100000</v>
+        <v>100001</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F4" s="8">
         <v>1</v>
@@ -10970,10 +10955,10 @@
         <v>100001</v>
       </c>
       <c r="D5" s="8">
-        <v>200000</v>
+        <v>200001</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F5" s="8">
         <v>1</v>
@@ -10984,13 +10969,13 @@
         <v>12</v>
       </c>
       <c r="C6" s="8">
-        <v>200000</v>
+        <v>200001</v>
       </c>
       <c r="D6" s="8">
         <v>100000000</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F6" s="33">
         <v>1</v>

</xml_diff>